<commit_message>
[LAF] base game #1
</commit_message>
<xml_diff>
--- a/Document/line_and_free_game_v3.xlsx
+++ b/Document/line_and_free_game_v3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SlotSimulation\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04A36E91-35B1-45A5-8EBE-F77E04CA05F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B3AEC9-1C47-4720-B4EA-CBC7A08B4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25665" yWindow="0" windowWidth="26040" windowHeight="20985" activeTab="1" xr2:uid="{85F1ABA9-DE8E-4950-9650-66A930469619}"/>
+    <workbookView xWindow="6540" yWindow="2010" windowWidth="30465" windowHeight="17550" activeTab="2" xr2:uid="{85F1ABA9-DE8E-4950-9650-66A930469619}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="4" r:id="rId1"/>
     <sheet name="Pay Table" sheetId="3" r:id="rId2"/>
-    <sheet name="Base Reel" sheetId="1" r:id="rId3"/>
+    <sheet name="Base Game Reel" sheetId="1" r:id="rId3"/>
     <sheet name="Free Game Reel" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -295,8 +295,8 @@
     <numFmt numFmtId="177" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="0.0000000"/>
-    <numFmt numFmtId="181" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="185" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -540,31 +540,16 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -581,6 +566,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61ECFED-FDEB-460A-9D88-C9A979303FD6}">
   <dimension ref="B3:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -990,178 +990,178 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="28" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="29">
         <v>300</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="29">
         <v>100</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="29">
         <v>250</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="29">
         <v>80</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="29">
         <v>100</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="29">
         <v>50</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="34">
+      <c r="B8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="29">
         <v>100</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="29">
         <v>50</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="34">
+      <c r="B9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="29">
         <v>80</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="29">
         <v>30</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="29">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="34">
+      <c r="B10" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="29">
         <v>50</v>
       </c>
-      <c r="D10" s="34">
-        <v>15</v>
-      </c>
-      <c r="E10" s="34">
+      <c r="D10" s="29">
+        <v>15</v>
+      </c>
+      <c r="E10" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="34">
+      <c r="B11" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="29">
         <v>25</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="29">
         <v>10</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="34">
+      <c r="B12" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="29">
         <v>25</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="29">
         <v>10</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="34">
+      <c r="B13" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="29">
         <v>25</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="29">
         <v>10</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="34">
+      <c r="B14" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="29">
         <v>25</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="29">
         <v>10</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="37">
+      <c r="B15" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="32">
         <v>20</v>
       </c>
-      <c r="D15" s="37">
-        <v>15</v>
-      </c>
-      <c r="E15" s="37">
+      <c r="D15" s="32">
+        <v>15</v>
+      </c>
+      <c r="E15" s="32">
         <v>10</v>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD34BBB1-4271-466A-86C7-92B04A304A75}">
   <dimension ref="B3:V125"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D70" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q107" sqref="Q107"/>
     </sheetView>
   </sheetViews>
@@ -1822,11 +1822,11 @@
       <c r="L17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="24">
+      <c r="M17" s="33">
         <f>PRODUCT(J16:N16)</f>
         <v>6272640000</v>
       </c>
-      <c r="N17" s="25"/>
+      <c r="N17" s="34"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
@@ -2903,13 +2903,13 @@
       <c r="G46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="26" t="s">
+      <c r="I46" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
       <c r="N46" s="9" t="s">
         <v>54</v>
       </c>
@@ -5209,13 +5209,13 @@
       <c r="I83" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J83" s="27" t="s">
+      <c r="J83" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="K83" s="27"/>
-      <c r="L83" s="27"/>
-      <c r="M83" s="27"/>
-      <c r="N83" s="28"/>
+      <c r="K83" s="36"/>
+      <c r="L83" s="36"/>
+      <c r="M83" s="36"/>
+      <c r="N83" s="37"/>
       <c r="O83" s="8" t="s">
         <v>0</v>
       </c>
@@ -6359,7 +6359,7 @@
       <c r="S111" t="s">
         <v>69</v>
       </c>
-      <c r="T111" s="29">
+      <c r="T111" s="24">
         <f>V77+U108</f>
         <v>0.27745870478777673</v>
       </c>
@@ -6378,7 +6378,7 @@
       <c r="S112" t="s">
         <v>70</v>
       </c>
-      <c r="T112" s="29">
+      <c r="T112" s="24">
         <f>'Free Game Reel'!W110</f>
         <v>10.549870146988539</v>
       </c>
@@ -7076,11 +7076,11 @@
       <c r="L17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="24">
+      <c r="M17" s="33">
         <f>PRODUCT(J16:N16)</f>
         <v>6159110400</v>
       </c>
-      <c r="N17" s="25"/>
+      <c r="N17" s="34"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
@@ -8157,13 +8157,13 @@
       <c r="G46" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="26" t="s">
+      <c r="I46" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
       <c r="N46" s="17" t="s">
         <v>54</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>4</v>
       </c>
       <c r="R58" s="1">
-        <f t="shared" ref="R57:R66" si="34">N34</f>
+        <f t="shared" ref="R58:R66" si="34">N34</f>
         <v>105</v>
       </c>
       <c r="S58" s="12">
@@ -10444,13 +10444,13 @@
       <c r="I82" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J82" s="27" t="s">
+      <c r="J82" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="K82" s="27"/>
-      <c r="L82" s="27"/>
-      <c r="M82" s="27"/>
-      <c r="N82" s="28"/>
+      <c r="K82" s="36"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="36"/>
+      <c r="N82" s="37"/>
       <c r="O82" s="8" t="s">
         <v>0</v>
       </c>
@@ -11462,7 +11462,7 @@
       <c r="U102" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="V102" s="31" t="s">
+      <c r="V102" s="26" t="s">
         <v>68</v>
       </c>
     </row>
@@ -11492,18 +11492,18 @@
         <f>SUM(T82:T91)</f>
         <v>226290375</v>
       </c>
-      <c r="T103" s="32">
+      <c r="T103" s="27">
         <f>SUM(U82:U91)</f>
         <v>3.6740756424823946E-2</v>
       </c>
       <c r="U103" s="1">
         <v>10</v>
       </c>
-      <c r="V103" s="29">
+      <c r="V103" s="24">
         <f>U103/$U$108</f>
         <v>10.396524989629299</v>
       </c>
-      <c r="W103" s="30">
+      <c r="W103" s="25">
         <f>V103*$V$77</f>
         <v>2.2953531864661869</v>
       </c>
@@ -11535,18 +11535,18 @@
         <f>SUM(T93:T97)</f>
         <v>16706250</v>
       </c>
-      <c r="T104" s="32">
+      <c r="T104" s="27">
         <f>SUM(U83:U92)</f>
         <v>4.1014912640630695E-2</v>
       </c>
       <c r="U104" s="1">
         <v>15</v>
       </c>
-      <c r="V104" s="29">
+      <c r="V104" s="24">
         <f>U104/$U$108</f>
         <v>15.594787484443948</v>
       </c>
-      <c r="W104" s="30">
+      <c r="W104" s="25">
         <f t="shared" ref="W104:W105" si="60">V104*$V$77</f>
         <v>3.4430297796992808</v>
       </c>
@@ -11568,18 +11568,18 @@
         <f>T100</f>
         <v>759375</v>
       </c>
-      <c r="T105" s="32">
+      <c r="T105" s="27">
         <f>SUM(U84:U93)</f>
         <v>3.6683767675279859E-2</v>
       </c>
       <c r="U105" s="1">
         <v>20</v>
       </c>
-      <c r="V105" s="29">
+      <c r="V105" s="24">
         <f>U105/$U$108</f>
         <v>20.793049979258598</v>
       </c>
-      <c r="W105" s="30">
+      <c r="W105" s="25">
         <f t="shared" si="60"/>
         <v>4.5907063729323738</v>
       </c>
@@ -11596,7 +11596,7 @@
       </c>
       <c r="T106" s="18"/>
       <c r="U106" s="1"/>
-      <c r="W106" s="30">
+      <c r="W106" s="25">
         <f>SUM(W103:W105)</f>
         <v>10.329089339097841</v>
       </c>
@@ -11653,7 +11653,7 @@
       <c r="G110" t="s">
         <v>12</v>
       </c>
-      <c r="W110" s="29">
+      <c r="W110" s="24">
         <f>V77+W106</f>
         <v>10.549870146988539</v>
       </c>

</xml_diff>